<commit_message>
filter() method for featureGroupsSet and negate support for features method
</commit_message>
<xml_diff>
--- a/set-impl.xlsx
+++ b/set-impl.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rick Helmus\Documents\Rproj\patRoon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C71DA90-119D-4AA3-ADF2-9BAA60992C06}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B886F0-D230-4717-9817-A03D43B2CF99}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4BFC050C-E8D8-4737-B5F4-2349612CBF83}"/>
+    <workbookView xWindow="25800" yWindow="0" windowWidth="25800" windowHeight="21000" xr2:uid="{4BFC050C-E8D8-4737-B5F4-2349612CBF83}"/>
   </bookViews>
   <sheets>
     <sheet name="fGroups" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="60">
   <si>
     <t>[</t>
   </si>
@@ -208,6 +208,9 @@
   </si>
   <si>
     <t>ionize</t>
+  </si>
+  <si>
+    <t>maybe wait for autoID branch</t>
   </si>
 </sst>
 </file>
@@ -559,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{577E9359-1D15-4F03-932A-97D98DDBC554}">
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -654,13 +657,19 @@
       <c r="C7" t="s">
         <v>49</v>
       </c>
+      <c r="G7" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>49</v>
+      </c>
+      <c r="G8" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -697,12 +706,18 @@
       <c r="F12" t="s">
         <v>49</v>
       </c>
+      <c r="G12" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
+        <v>49</v>
+      </c>
+      <c r="G13" t="s">
         <v>49</v>
       </c>
     </row>
@@ -713,6 +728,9 @@
       <c r="C14" t="s">
         <v>49</v>
       </c>
+      <c r="G14" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -730,7 +748,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -738,7 +756,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -746,7 +764,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -757,7 +775,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -765,7 +783,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -773,7 +791,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -784,23 +802,26 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
       <c r="D23" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
       </c>
-      <c r="C24" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G24" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -811,7 +832,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -822,7 +843,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -833,7 +854,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -844,7 +865,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -855,31 +876,40 @@
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="G30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="G31" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>29</v>
       </c>
       <c r="B32" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G32" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>30</v>
       </c>
@@ -887,47 +917,62 @@
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>31</v>
       </c>
       <c r="B34" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="G34" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>32</v>
       </c>
       <c r="B35" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G35" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>33</v>
       </c>
       <c r="B36" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G36" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>34</v>
       </c>
       <c r="B37" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G37" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>35</v>
       </c>
       <c r="B38" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G38" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>36</v>
       </c>
@@ -938,7 +983,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>37</v>
       </c>
@@ -949,7 +994,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>38</v>
       </c>
@@ -960,7 +1005,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>39</v>
       </c>
@@ -971,7 +1016,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>40</v>
       </c>
@@ -982,15 +1027,18 @@
         <v>49</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>41</v>
       </c>
       <c r="B44" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="G44" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>42</v>
       </c>
@@ -998,7 +1046,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>43</v>
       </c>
@@ -1006,7 +1054,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>44</v>
       </c>
@@ -1014,12 +1062,15 @@
         <v>49</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>45</v>
       </c>
       <c r="D48" t="s">
         <v>49</v>
+      </c>
+      <c r="H48" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -1038,7 +1089,10 @@
         <v>47</v>
       </c>
       <c r="B50" t="s">
-        <v>53</v>
+        <v>49</v>
+      </c>
+      <c r="G50" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -1046,7 +1100,10 @@
         <v>55</v>
       </c>
       <c r="B51" t="s">
-        <v>53</v>
+        <v>49</v>
+      </c>
+      <c r="G51" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -1054,6 +1111,9 @@
         <v>56</v>
       </c>
       <c r="D53" t="s">
+        <v>49</v>
+      </c>
+      <c r="G53" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>

<commit_message>
plotEIC methods for fGroupsSet
</commit_message>
<xml_diff>
--- a/set-impl.xlsx
+++ b/set-impl.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rick Helmus\Documents\Rproj\patRoon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B886F0-D230-4717-9817-A03D43B2CF99}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11A24ECB-3AC7-4C4A-93D5-048489AB0E3F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25800" yWindow="0" windowWidth="25800" windowHeight="21000" xr2:uid="{4BFC050C-E8D8-4737-B5F4-2349612CBF83}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="61">
   <si>
     <t>[</t>
   </si>
@@ -211,6 +211,9 @@
   </si>
   <si>
     <t>maybe wait for autoID branch</t>
+  </si>
+  <si>
+    <t>getEICsForFGroups</t>
   </si>
 </sst>
 </file>
@@ -562,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{577E9359-1D15-4F03-932A-97D98DDBC554}">
-  <dimension ref="A1:H53"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,9 +769,12 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" t="s">
         <v>49</v>
       </c>
       <c r="G19" t="s">
@@ -777,15 +783,18 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>49</v>
+      </c>
+      <c r="G20" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E21" t="s">
         <v>49</v>
@@ -793,40 +802,37 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" t="s">
-        <v>49</v>
-      </c>
-      <c r="G22" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" t="s">
-        <v>53</v>
-      </c>
-      <c r="H23" t="s">
-        <v>59</v>
+        <v>19</v>
+      </c>
+      <c r="B23" t="s">
+        <v>49</v>
+      </c>
+      <c r="G23" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>21</v>
-      </c>
-      <c r="G24" t="s">
-        <v>49</v>
+        <v>20</v>
+      </c>
+      <c r="D24" t="s">
+        <v>53</v>
+      </c>
+      <c r="H24" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="G25" t="s">
         <v>49</v>
@@ -834,7 +840,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B26" t="s">
         <v>49</v>
@@ -845,9 +851,9 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>24</v>
-      </c>
-      <c r="C27" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" t="s">
         <v>49</v>
       </c>
       <c r="G27" t="s">
@@ -856,9 +862,9 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>25</v>
-      </c>
-      <c r="B28" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" t="s">
         <v>49</v>
       </c>
       <c r="G28" t="s">
@@ -867,7 +873,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B29" t="s">
         <v>49</v>
@@ -878,7 +884,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B30" t="s">
         <v>49</v>
@@ -889,7 +895,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B31" t="s">
         <v>49</v>
@@ -900,220 +906,234 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" t="s">
+        <v>49</v>
+      </c>
+      <c r="G32" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>29</v>
       </c>
-      <c r="B32" t="s">
-        <v>49</v>
-      </c>
-      <c r="G32" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="B33" t="s">
+        <v>49</v>
+      </c>
+      <c r="G33" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>30</v>
       </c>
-      <c r="D33" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="D34" t="s">
+        <v>49</v>
+      </c>
+      <c r="G34" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>31</v>
       </c>
-      <c r="B34" t="s">
-        <v>49</v>
-      </c>
-      <c r="G34" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="B35" t="s">
+        <v>49</v>
+      </c>
+      <c r="G35" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>32</v>
       </c>
-      <c r="B35" t="s">
-        <v>49</v>
-      </c>
-      <c r="G35" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="B36" t="s">
+        <v>49</v>
+      </c>
+      <c r="G36" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>33</v>
       </c>
-      <c r="B36" t="s">
-        <v>49</v>
-      </c>
-      <c r="G36" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="B37" t="s">
+        <v>49</v>
+      </c>
+      <c r="G37" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>34</v>
       </c>
-      <c r="B37" t="s">
-        <v>49</v>
-      </c>
-      <c r="G37" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="B38" t="s">
+        <v>49</v>
+      </c>
+      <c r="G38" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>35</v>
       </c>
-      <c r="B38" t="s">
-        <v>49</v>
-      </c>
-      <c r="G38" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="B39" t="s">
+        <v>49</v>
+      </c>
+      <c r="G39" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>36</v>
       </c>
-      <c r="B39" t="s">
-        <v>49</v>
-      </c>
-      <c r="G39" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="B40" t="s">
+        <v>49</v>
+      </c>
+      <c r="G40" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>37</v>
       </c>
-      <c r="B40" t="s">
-        <v>49</v>
-      </c>
-      <c r="G40" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="B41" t="s">
+        <v>49</v>
+      </c>
+      <c r="G41" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>38</v>
       </c>
-      <c r="B41" t="s">
-        <v>49</v>
-      </c>
-      <c r="G41" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="B42" t="s">
+        <v>49</v>
+      </c>
+      <c r="G42" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>39</v>
       </c>
-      <c r="B42" t="s">
-        <v>49</v>
-      </c>
-      <c r="G42" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="B43" t="s">
+        <v>49</v>
+      </c>
+      <c r="G43" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>40</v>
       </c>
-      <c r="B43" t="s">
-        <v>49</v>
-      </c>
-      <c r="G43" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="B44" t="s">
+        <v>49</v>
+      </c>
+      <c r="G44" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>41</v>
       </c>
-      <c r="B44" t="s">
-        <v>49</v>
-      </c>
-      <c r="G44" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="B45" t="s">
+        <v>49</v>
+      </c>
+      <c r="G45" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>42</v>
       </c>
-      <c r="D45" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="D46" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>43</v>
       </c>
-      <c r="D46" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="D47" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>44</v>
       </c>
-      <c r="D47" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="D48" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>45</v>
       </c>
-      <c r="D48" t="s">
-        <v>49</v>
-      </c>
-      <c r="H48" t="s">
+      <c r="D49" t="s">
+        <v>49</v>
+      </c>
+      <c r="H49" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>46</v>
       </c>
-      <c r="C49" t="s">
-        <v>49</v>
-      </c>
-      <c r="G49" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="C50" t="s">
+        <v>49</v>
+      </c>
+      <c r="G50" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>47</v>
       </c>
-      <c r="B50" t="s">
-        <v>49</v>
-      </c>
-      <c r="G50" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="B51" t="s">
+        <v>49</v>
+      </c>
+      <c r="G51" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>55</v>
       </c>
-      <c r="B51" t="s">
-        <v>49</v>
-      </c>
-      <c r="G51" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="B52" t="s">
+        <v>49</v>
+      </c>
+      <c r="G52" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>56</v>
       </c>
-      <c r="D53" t="s">
-        <v>49</v>
-      </c>
-      <c r="G53" t="s">
+      <c r="D54" t="s">
+        <v>49</v>
+      </c>
+      <c r="G54" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>

<commit_message>
started on set MSPeakLists
</commit_message>
<xml_diff>
--- a/set-impl.xlsx
+++ b/set-impl.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rick Helmus\Documents\Rproj\patRoon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11A24ECB-3AC7-4C4A-93D5-048489AB0E3F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{333046D1-D61A-4874-A391-2A9E64332933}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25800" yWindow="0" windowWidth="25800" windowHeight="21000" xr2:uid="{4BFC050C-E8D8-4737-B5F4-2349612CBF83}"/>
+    <workbookView xWindow="25800" yWindow="0" windowWidth="25800" windowHeight="21000" activeTab="1" xr2:uid="{4BFC050C-E8D8-4737-B5F4-2349612CBF83}"/>
   </bookViews>
   <sheets>
     <sheet name="fGroups" sheetId="1" r:id="rId1"/>
+    <sheet name="mslists" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="64">
   <si>
     <t>[</t>
   </si>
@@ -214,13 +215,22 @@
   </si>
   <si>
     <t>getEICsForFGroups</t>
+  </si>
+  <si>
+    <t>averagedPeakLists</t>
+  </si>
+  <si>
+    <t>peakLists</t>
+  </si>
+  <si>
+    <t>plotSpec</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -228,13 +238,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Fira Code"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -249,8 +271,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -567,8 +595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{577E9359-1D15-4F03-932A-97D98DDBC554}">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1140,4 +1168,158 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8FAD30B-F556-40FF-A251-17FA26BFE1EF}">
+  <dimension ref="A1:G15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ionization and [[ for MSPeakListsSet
</commit_message>
<xml_diff>
--- a/set-impl.xlsx
+++ b/set-impl.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rick Helmus\Documents\Rproj\patRoon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C10E1C-7095-4D38-80CA-747194175699}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DACA4F2D-B542-463A-BAF8-42588E366F80}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25800" yWindow="0" windowWidth="25800" windowHeight="21000" activeTab="1" xr2:uid="{4BFC050C-E8D8-4737-B5F4-2349612CBF83}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="64">
   <si>
     <t>[</t>
   </si>
@@ -1178,7 +1178,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1235,6 +1235,12 @@
       <c r="C4" t="s">
         <v>49</v>
       </c>
+      <c r="F4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">

</xml_diff>

<commit_message>
peakList accessors for MSPeakListsSet
</commit_message>
<xml_diff>
--- a/set-impl.xlsx
+++ b/set-impl.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rick Helmus\Documents\Rproj\patRoon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E2208C-8FF8-4023-A8D8-05AF2F434394}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15612F53-16D8-4D09-B257-75CB7F68C3C5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25800" yWindow="0" windowWidth="25800" windowHeight="21000" activeTab="1" xr2:uid="{4BFC050C-E8D8-4737-B5F4-2349612CBF83}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="64">
   <si>
     <t>[</t>
   </si>
@@ -1178,7 +1178,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1277,6 +1277,12 @@
       <c r="C7" t="s">
         <v>49</v>
       </c>
+      <c r="F7" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -1301,6 +1307,9 @@
       <c r="B10" t="s">
         <v>49</v>
       </c>
+      <c r="G10" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -1309,6 +1318,9 @@
       <c r="C11" t="s">
         <v>49</v>
       </c>
+      <c r="G11" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -1317,12 +1329,21 @@
       <c r="B12" t="s">
         <v>49</v>
       </c>
+      <c r="G12" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>62</v>
       </c>
       <c r="C13" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" t="s">
+        <v>49</v>
+      </c>
+      <c r="G13" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>

<commit_message>
show() method for MSPeakListsSet
</commit_message>
<xml_diff>
--- a/set-impl.xlsx
+++ b/set-impl.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rick Helmus\Documents\Rproj\patRoon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15612F53-16D8-4D09-B257-75CB7F68C3C5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7A8B4D3-998A-4EE7-BA7D-415FFF8205A6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25800" yWindow="0" windowWidth="25800" windowHeight="21000" activeTab="1" xr2:uid="{4BFC050C-E8D8-4737-B5F4-2349612CBF83}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="64">
   <si>
     <t>[</t>
   </si>
@@ -1178,7 +1178,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1362,6 +1362,9 @@
       <c r="C15" t="s">
         <v>49</v>
       </c>
+      <c r="G15" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">

</xml_diff>

<commit_message>
WIP plotSpec() for MSPeakListsSet
</commit_message>
<xml_diff>
--- a/set-impl.xlsx
+++ b/set-impl.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rick Helmus\Documents\Rproj\patRoon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9173E7E8-819F-43B1-ACCC-701DDD952608}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88217751-2924-4EA5-AFAB-1DBB6CD2F5AD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25800" yWindow="0" windowWidth="25800" windowHeight="21000" activeTab="1" xr2:uid="{4BFC050C-E8D8-4737-B5F4-2349612CBF83}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="64">
   <si>
     <t>[</t>
   </si>
@@ -1178,7 +1178,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1357,6 +1357,9 @@
       <c r="B14" t="s">
         <v>53</v>
       </c>
+      <c r="F14" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">

</xml_diff>

<commit_message>
remove unneeded method override
</commit_message>
<xml_diff>
--- a/set-impl.xlsx
+++ b/set-impl.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rick Helmus\Documents\Rproj\patRoon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC07322C-E038-4EC4-B2EA-27113096F002}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{146D90B9-4CA8-4E79-B462-95B326E8A443}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25800" yWindow="0" windowWidth="25800" windowHeight="21000" activeTab="3" xr2:uid="{4BFC050C-E8D8-4737-B5F4-2349612CBF83}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="3" xr2:uid="{4BFC050C-E8D8-4737-B5F4-2349612CBF83}"/>
   </bookViews>
   <sheets>
     <sheet name="fGroups" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="80">
   <si>
     <t>[</t>
   </si>
@@ -1698,7 +1698,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1735,11 +1735,20 @@
       <c r="B2" t="s">
         <v>49</v>
       </c>
+      <c r="G2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="D3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -1748,6 +1757,9 @@
       <c r="B4" t="s">
         <v>53</v>
       </c>
+      <c r="G4" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -1764,6 +1776,9 @@
       <c r="B6" t="s">
         <v>49</v>
       </c>
+      <c r="G6" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -1777,7 +1792,10 @@
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C8" t="s">
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>

<commit_message>
plotSpec() method for compoundsSet and and necessary refactoring/clean-up of compounds plotSpec() method
</commit_message>
<xml_diff>
--- a/set-impl.xlsx
+++ b/set-impl.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rick Helmus\Documents\Rproj\patRoon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D0A2A73-87D0-4D07-BF1D-6EF7FF0D3202}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA502245-1AFA-4F81-8540-AA92E578E78F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="3" xr2:uid="{4BFC050C-E8D8-4737-B5F4-2349612CBF83}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="80">
   <si>
     <t>[</t>
   </si>
@@ -1698,7 +1698,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1850,6 +1850,9 @@
       <c r="B13" t="s">
         <v>49</v>
       </c>
+      <c r="G13" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
@@ -1900,7 +1903,10 @@
         <v>76</v>
       </c>
       <c r="B18" t="s">
-        <v>53</v>
+        <v>49</v>
+      </c>
+      <c r="G18" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1921,6 +1927,9 @@
       <c r="B20" t="s">
         <v>49</v>
       </c>
+      <c r="G20" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
@@ -1929,6 +1938,9 @@
       <c r="B21" t="s">
         <v>49</v>
       </c>
+      <c r="G21" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -1937,6 +1949,9 @@
       <c r="D22" t="s">
         <v>49</v>
       </c>
+      <c r="G22" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -1953,12 +1968,18 @@
       <c r="B24" t="s">
         <v>53</v>
       </c>
+      <c r="G24" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>79</v>
       </c>
       <c r="B25" t="s">
+        <v>49</v>
+      </c>
+      <c r="G25" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>

<commit_message>
generics for generation of set compounds
</commit_message>
<xml_diff>
--- a/set-impl.xlsx
+++ b/set-impl.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rick Helmus\Documents\Rproj\patRoon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B253293-B4C6-4EED-AB05-0F0CCF2600AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7B53F3-E7BC-4503-8221-5DAB77C6BECD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="2" xr2:uid="{4BFC050C-E8D8-4737-B5F4-2349612CBF83}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="3" xr2:uid="{4BFC050C-E8D8-4737-B5F4-2349612CBF83}"/>
   </bookViews>
   <sheets>
     <sheet name="fGroups" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="80">
   <si>
     <t>[</t>
   </si>
@@ -1436,7 +1436,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F55E5D-7D4A-4C47-B642-2945193FC9B1}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -1697,8 +1697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3D77136-34B2-4F7F-8663-E1F52F93A0FB}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1969,7 +1969,7 @@
         <v>78</v>
       </c>
       <c r="B24" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G24" t="s">
         <v>49</v>
@@ -1993,12 +1993,18 @@
       <c r="B26" t="s">
         <v>49</v>
       </c>
+      <c r="G26" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>35</v>
       </c>
       <c r="B27" t="s">
+        <v>49</v>
+      </c>
+      <c r="G27" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix subset method definition, remove unneeded plotSpec() override
</commit_message>
<xml_diff>
--- a/set-impl.xlsx
+++ b/set-impl.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rick Helmus\Documents\Rproj\patRoon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7B53F3-E7BC-4503-8221-5DAB77C6BECD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB881E3C-BFB4-49B4-B18C-5F88D9E6BFE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="3" xr2:uid="{4BFC050C-E8D8-4737-B5F4-2349612CBF83}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="1" activeTab="4" xr2:uid="{4BFC050C-E8D8-4737-B5F4-2349612CBF83}"/>
   </bookViews>
   <sheets>
     <sheet name="fGroups" sheetId="1" r:id="rId1"/>
     <sheet name="mslists" sheetId="2" r:id="rId2"/>
     <sheet name="formulas" sheetId="3" r:id="rId3"/>
     <sheet name="compounds" sheetId="4" r:id="rId4"/>
+    <sheet name="components" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="84">
   <si>
     <t>[</t>
   </si>
@@ -276,6 +277,18 @@
   </si>
   <si>
     <t>plotStructureHash</t>
+  </si>
+  <si>
+    <t>componentInfo</t>
+  </si>
+  <si>
+    <t>componentTable</t>
+  </si>
+  <si>
+    <t>findFGroup</t>
+  </si>
+  <si>
+    <t>Seems enough, assuming we're not planning to merge components</t>
   </si>
 </sst>
 </file>
@@ -1697,8 +1710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3D77136-34B2-4F7F-8663-E1F52F93A0FB}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2023,4 +2036,249 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D3C2673-B09C-47B8-945F-B7E3A2F3EE99}">
+  <dimension ref="A1:H19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>49</v>
+      </c>
+      <c r="G13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" t="s">
+        <v>49</v>
+      </c>
+      <c r="H15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" t="s">
+        <v>49</v>
+      </c>
+      <c r="G16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" t="s">
+        <v>49</v>
+      </c>
+      <c r="G17" t="s">
+        <v>49</v>
+      </c>
+      <c r="H17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+      <c r="G18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" t="s">
+        <v>49</v>
+      </c>
+      <c r="G19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
workflowStepSet base class for sets classes
</commit_message>
<xml_diff>
--- a/set-impl.xlsx
+++ b/set-impl.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rick Helmus\Documents\Rproj\patRoon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB881E3C-BFB4-49B4-B18C-5F88D9E6BFE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{733C23AC-FF14-4159-BD76-5A0F1A5E54BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="1" activeTab="4" xr2:uid="{4BFC050C-E8D8-4737-B5F4-2349612CBF83}"/>
+    <workbookView xWindow="25800" yWindow="0" windowWidth="3000" windowHeight="15600" firstSheet="1" activeTab="5" xr2:uid="{4BFC050C-E8D8-4737-B5F4-2349612CBF83}"/>
   </bookViews>
   <sheets>
     <sheet name="fGroups" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="formulas" sheetId="3" r:id="rId3"/>
     <sheet name="compounds" sheetId="4" r:id="rId4"/>
     <sheet name="components" sheetId="5" r:id="rId5"/>
+    <sheet name="classes" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="95">
   <si>
     <t>[</t>
   </si>
@@ -289,6 +290,39 @@
   </si>
   <si>
     <t>Seems enough, assuming we're not planning to merge components</t>
+  </si>
+  <si>
+    <t>featuresSet</t>
+  </si>
+  <si>
+    <t>adducts</t>
+  </si>
+  <si>
+    <t>setObjects</t>
+  </si>
+  <si>
+    <t>ionizedXXX</t>
+  </si>
+  <si>
+    <t>featuresGroupsSet</t>
+  </si>
+  <si>
+    <t>MSPeakListsSet</t>
+  </si>
+  <si>
+    <t>formulasSet</t>
+  </si>
+  <si>
+    <t>compoundsSet</t>
+  </si>
+  <si>
+    <t>componentsSet</t>
+  </si>
+  <si>
+    <t>setThreshold</t>
+  </si>
+  <si>
+    <t>origFGNames</t>
   </si>
 </sst>
 </file>
@@ -336,7 +370,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -352,6 +386,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2042,7 +2079,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D3C2673-B09C-47B8-945F-B7E3A2F3EE99}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
@@ -2281,4 +2318,175 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1CF8BB5-F733-42C2-A946-991B96C9C1B3}">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>